<commit_message>
changed scheduled from fifteen minutes to thirty
</commit_message>
<xml_diff>
--- a/data/excel files/out/adw.xlsx
+++ b/data/excel files/out/adw.xlsx
@@ -208,7 +208,7 @@
     <t>BEAST</t>
   </si>
   <si>
-    <t>TWOFACE</t>
+    <t>TWO-FACE</t>
   </si>
   <si>
     <t>WINGKIT</t>
@@ -607,11 +607,11 @@
     <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="18" max="32" width="3.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>